<commit_message>
update chnpp upload utils
</commit_message>
<xml_diff>
--- a/wdc_libs/ssechnpp-utils/new data/SSMS_DAU_RLD.xlsx
+++ b/wdc_libs/ssechnpp-utils/new data/SSMS_DAU_RLD.xlsx
@@ -206,7 +206,7 @@
 line(x:-1);</t>
   </si>
   <si>
-    <t>SSMS-DAU-004-RLD302-VAL*.CSV</t>
+    <t>SSMS-DAU004-RLD302-VAL*.CSV</t>
   </si>
 </sst>
 </file>
@@ -548,7 +548,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -559,7 +559,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>